<commit_message>
readme and notebook update
</commit_message>
<xml_diff>
--- a/examples/sample_data/colocalization_cfos_tdt/colocalization_results.xlsx
+++ b/examples/sample_data/colocalization_cfos_tdt/colocalization_results.xlsx
@@ -452,7 +452,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3">
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4">
@@ -472,7 +472,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5">
@@ -482,7 +482,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>